<commit_message>
Añadido de página de dashboard con estadisticas de los tickets
</commit_message>
<xml_diff>
--- a/[docs]/Apuntes DER database.xlsx
+++ b/[docs]/Apuntes DER database.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\lcorrea\Desktop\Salchy\UTN\[proyectos]\HelpFlow\[docs]\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FD607EBB-8DE7-467F-8D7B-74664E32E50A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D2C40784-7C47-49BF-860D-3647FFCF980A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="20370" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Categorías de Tickets" sheetId="2" r:id="rId1"/>
@@ -27,10 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="44" uniqueCount="44">
-  <si>
-    <t>Incidencias / Errores</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="46" uniqueCount="45">
   <si>
     <t>Problemas de hardware</t>
   </si>
@@ -89,9 +86,6 @@
     <t>Configuraciones especiales</t>
   </si>
   <si>
-    <t>Integraciones entre sistemas</t>
-  </si>
-  <si>
     <t>Mantenimiento Preventivo / Correctivo</t>
   </si>
   <si>
@@ -134,9 +128,6 @@
     <t>Sugerencias sobre sistemas o infraestructura</t>
   </si>
   <si>
-    <t>Abierto</t>
-  </si>
-  <si>
     <t>En progreso</t>
   </si>
   <si>
@@ -159,6 +150,18 @@
   </si>
   <si>
     <t>Usuario Usuario</t>
+  </si>
+  <si>
+    <t>Solicitud</t>
+  </si>
+  <si>
+    <t>Categoria</t>
+  </si>
+  <si>
+    <t>_</t>
+  </si>
+  <si>
+    <t>Sub Categoria</t>
   </si>
 </sst>
 </file>
@@ -495,10 +498,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5A1EF922-C7C9-4C4B-9F67-D62C44B44456}">
-  <dimension ref="A2:B36"/>
+  <dimension ref="A1:B36"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C35" sqref="C35"/>
+      <selection activeCell="B6" sqref="B6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -507,179 +510,187 @@
     <col min="2" max="2" width="41" style="2" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>42</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>44</v>
+      </c>
+    </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" s="3" t="s">
-        <v>0</v>
+        <v>43</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B3" s="2" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B4" s="2" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B5" s="2" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B6" s="2" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B7" s="1" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A8" s="3" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B9" s="2" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B10" s="2" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B11" s="2" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A12" s="3" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B13" s="2" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B14" s="2" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
     </row>
     <row r="15" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B15" s="2" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
     </row>
     <row r="16" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B16" s="2" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B17" s="2" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
     <row r="18" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A18" s="3" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
     </row>
     <row r="19" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B19" s="2" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="20" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B20" s="2" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
     </row>
     <row r="21" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B21" s="2" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="22" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A22" s="3" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="22" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="B22" s="2" t="s">
+    <row r="23" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B23" s="2" t="s">
         <v>20</v>
-      </c>
-    </row>
-    <row r="23" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A23" s="3" t="s">
-        <v>21</v>
       </c>
     </row>
     <row r="24" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B24" s="2" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
     </row>
     <row r="25" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B25" s="2" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
     </row>
     <row r="26" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B26" s="2" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="27" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A27" s="3" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="27" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="B27" s="2" t="s">
+    <row r="28" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B28" s="2" t="s">
         <v>25</v>
-      </c>
-    </row>
-    <row r="28" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A28" s="3" t="s">
-        <v>26</v>
       </c>
     </row>
     <row r="29" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B29" s="2" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
     </row>
     <row r="30" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B30" s="2" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="31" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B31" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="31" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="B31" s="2" t="s">
+    <row r="32" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A32" s="4" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="32" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="B32" t="s">
+    <row r="33" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B33" s="2" t="s">
         <v>30</v>
       </c>
     </row>
-    <row r="33" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A33" s="4" t="s">
+    <row r="34" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B34" s="2" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="34" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="B34" s="2" t="s">
+    <row r="35" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B35" s="2" t="s">
         <v>32</v>
       </c>
     </row>
-    <row r="35" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="B35" s="2" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="36" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="36" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B36" s="2" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
     </row>
   </sheetData>
@@ -692,14 +703,14 @@
   <dimension ref="A1:B7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A6" sqref="A6"/>
+      <selection activeCell="C39" sqref="C39"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>39</v>
+        <v>36</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
@@ -707,7 +718,7 @@
         <v>0</v>
       </c>
       <c r="B2" t="s">
-        <v>35</v>
+        <v>41</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
@@ -715,7 +726,7 @@
         <v>1</v>
       </c>
       <c r="B3" t="s">
-        <v>36</v>
+        <v>33</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
@@ -723,7 +734,7 @@
         <v>2</v>
       </c>
       <c r="B4" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.25">
@@ -731,7 +742,7 @@
         <v>3</v>
       </c>
       <c r="B5" t="s">
-        <v>38</v>
+        <v>35</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.25">
@@ -757,10 +768,10 @@
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
       <c r="B1" t="s">
-        <v>41</v>
+        <v>38</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
@@ -768,7 +779,7 @@
         <v>0</v>
       </c>
       <c r="B2" t="s">
-        <v>42</v>
+        <v>39</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
@@ -776,7 +787,7 @@
         <v>1</v>
       </c>
       <c r="B3" t="s">
-        <v>43</v>
+        <v>40</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Modificación de esquema de Base de Datos, para añadir tablas Categorias y SubCategorias
</commit_message>
<xml_diff>
--- a/[docs]/Apuntes DER database.xlsx
+++ b/[docs]/Apuntes DER database.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\lcorrea\Desktop\Salchy\UTN\[proyectos]\HelpFlow\[docs]\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D2C40784-7C47-49BF-860D-3647FFCF980A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C81F0256-0608-48C5-8887-598350EA6682}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="20370" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -27,7 +27,10 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="46" uniqueCount="45">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="45" uniqueCount="45">
+  <si>
+    <t>Incidencias / Errores</t>
+  </si>
   <si>
     <t>Problemas de hardware</t>
   </si>
@@ -158,10 +161,7 @@
     <t>Categoria</t>
   </si>
   <si>
-    <t>_</t>
-  </si>
-  <si>
-    <t>Sub Categoria</t>
+    <t>SubCategoria</t>
   </si>
 </sst>
 </file>
@@ -498,10 +498,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5A1EF922-C7C9-4C4B-9F67-D62C44B44456}">
-  <dimension ref="A1:B36"/>
+  <dimension ref="A1:B35"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B6" sqref="B6"/>
+      <selection activeCell="E30" sqref="E30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -512,7 +512,7 @@
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="B1" s="2" t="s">
         <v>44</v>
@@ -520,177 +520,172 @@
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" s="3" t="s">
-        <v>43</v>
+        <v>0</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B3" s="2" t="s">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B4" s="2" t="s">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B5" s="2" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B6" s="2" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B7" s="1" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A8" s="3" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B9" s="2" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B10" s="2" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B11" s="2" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A12" s="3" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B13" s="2" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B14" s="2" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
     </row>
     <row r="15" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B15" s="2" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
     </row>
     <row r="16" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B16" s="2" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B17" s="2" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
     </row>
     <row r="18" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A18" s="3" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
     </row>
     <row r="19" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B19" s="2" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
     </row>
     <row r="20" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B20" s="2" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
     </row>
     <row r="21" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B21" s="2" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
     </row>
     <row r="22" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A22" s="3" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
     </row>
     <row r="23" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B23" s="2" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
     </row>
     <row r="24" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B24" s="2" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
     </row>
     <row r="25" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B25" s="2" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
     </row>
     <row r="26" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B26" s="2" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
     </row>
     <row r="27" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A27" s="3" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
     </row>
     <row r="28" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B28" s="2" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
     </row>
     <row r="29" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B29" s="2" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
     </row>
     <row r="30" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B30" s="2" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
     </row>
     <row r="31" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B31" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
     </row>
     <row r="32" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A32" s="4" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
     </row>
     <row r="33" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B33" s="2" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
     </row>
     <row r="34" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B34" s="2" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
     </row>
     <row r="35" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B35" s="2" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="36" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B36" s="2" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
     </row>
   </sheetData>
@@ -710,7 +705,7 @@
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
@@ -718,7 +713,7 @@
         <v>0</v>
       </c>
       <c r="B2" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
@@ -726,7 +721,7 @@
         <v>1</v>
       </c>
       <c r="B3" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
@@ -734,7 +729,7 @@
         <v>2</v>
       </c>
       <c r="B4" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.25">
@@ -742,7 +737,7 @@
         <v>3</v>
       </c>
       <c r="B5" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.25">
@@ -768,10 +763,10 @@
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="B1" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
@@ -779,7 +774,7 @@
         <v>0</v>
       </c>
       <c r="B2" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
@@ -787,7 +782,7 @@
         <v>1</v>
       </c>
       <c r="B3" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Arreglos en visual de listado de tickets + Insert de datos de prueba
</commit_message>
<xml_diff>
--- a/[docs]/Apuntes DER database.xlsx
+++ b/[docs]/Apuntes DER database.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\lcorrea\Desktop\Salchy\UTN\[proyectos]\HelpFlow\[docs]\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C81F0256-0608-48C5-8887-598350EA6682}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ACE90415-848E-4975-A75E-B7012470AE12}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="20370" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="45" uniqueCount="45">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="46" uniqueCount="46">
   <si>
     <t>Incidencias / Errores</t>
   </si>
@@ -158,10 +158,13 @@
     <t>Solicitud</t>
   </si>
   <si>
-    <t>Categoria</t>
-  </si>
-  <si>
     <t>SubCategoria</t>
+  </si>
+  <si>
+    <t>Id 1</t>
+  </si>
+  <si>
+    <t>id 2</t>
   </si>
 </sst>
 </file>
@@ -205,7 +208,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
@@ -218,6 +221,15 @@
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="15" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -498,193 +510,312 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5A1EF922-C7C9-4C4B-9F67-D62C44B44456}">
-  <dimension ref="A1:B35"/>
+  <dimension ref="A1:D35"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E30" sqref="E30"/>
+      <selection activeCell="I36" sqref="I36"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="36.42578125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="41" style="2" bestFit="1" customWidth="1"/>
+    <col min="1" max="2" width="4.140625" style="6" bestFit="1" customWidth="1"/>
+    <col min="3" max="4" width="41" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A1" t="s">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A1" s="6" t="s">
+        <v>44</v>
+      </c>
+      <c r="B1" s="6" t="s">
+        <v>45</v>
+      </c>
+      <c r="C1" s="2" t="s">
         <v>43</v>
       </c>
-      <c r="B1" s="2" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A2" s="3" t="s">
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A2" s="7">
+        <v>1</v>
+      </c>
+      <c r="B2" s="7"/>
+      <c r="C2" s="3" t="s">
         <v>0</v>
       </c>
-    </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="B3" s="2" t="s">
+      <c r="D2" s="2"/>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B3" s="6">
         <v>1</v>
       </c>
-    </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="B4" s="2" t="s">
+      <c r="D3" s="2" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B4" s="6">
         <v>2</v>
       </c>
-    </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="B5" s="2" t="s">
+      <c r="D4" s="2" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B5" s="6">
         <v>3</v>
       </c>
-    </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="B6" s="2" t="s">
+      <c r="D5" s="2" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B6" s="6">
         <v>4</v>
       </c>
-    </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="B7" s="1" t="s">
+      <c r="D6" s="2" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B7" s="6">
         <v>5</v>
       </c>
-    </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A8" s="3" t="s">
+      <c r="D7" s="1" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A8" s="7">
+        <v>2</v>
+      </c>
+      <c r="B8" s="7"/>
+      <c r="C8" s="3" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="B9" s="2" t="s">
+      <c r="D8" s="2"/>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B9" s="6">
+        <v>6</v>
+      </c>
+      <c r="D9" s="2" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="B10" s="2" t="s">
+    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B10" s="6">
+        <v>7</v>
+      </c>
+      <c r="D10" s="2" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="B11" s="2" t="s">
+    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B11" s="6">
+        <v>8</v>
+      </c>
+      <c r="D11" s="2" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A12" s="3" t="s">
+    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A12" s="7">
+        <v>3</v>
+      </c>
+      <c r="B12" s="7"/>
+      <c r="C12" s="3" t="s">
         <v>10</v>
       </c>
-    </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="B13" s="2" t="s">
+      <c r="D12" s="2"/>
+    </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B13" s="6">
+        <v>9</v>
+      </c>
+      <c r="D13" s="2" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="14" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="B14" s="2" t="s">
+    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B14" s="6">
+        <v>10</v>
+      </c>
+      <c r="D14" s="2" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="15" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="B15" s="2" t="s">
+    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B15" s="6">
+        <v>11</v>
+      </c>
+      <c r="D15" s="2" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="16" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="B16" s="2" t="s">
+    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B16" s="6">
+        <v>12</v>
+      </c>
+      <c r="D16" s="2" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="B17" s="2" t="s">
+    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B17" s="6">
+        <v>13</v>
+      </c>
+      <c r="D17" s="2" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A18" s="3" t="s">
+    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A18" s="7">
+        <v>4</v>
+      </c>
+      <c r="B18" s="7"/>
+      <c r="C18" s="3" t="s">
         <v>16</v>
       </c>
-    </row>
-    <row r="19" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="B19" s="2" t="s">
+      <c r="D18" s="2"/>
+    </row>
+    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B19" s="6">
+        <v>14</v>
+      </c>
+      <c r="D19" s="2" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="20" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="B20" s="2" t="s">
+    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B20" s="6">
+        <v>15</v>
+      </c>
+      <c r="D20" s="2" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="21" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="B21" s="2" t="s">
+    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B21" s="6">
+        <v>16</v>
+      </c>
+      <c r="D21" s="2" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="22" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A22" s="3" t="s">
+    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A22" s="7">
+        <v>5</v>
+      </c>
+      <c r="B22" s="7"/>
+      <c r="C22" s="3" t="s">
         <v>20</v>
       </c>
-    </row>
-    <row r="23" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="B23" s="2" t="s">
+      <c r="D22" s="2"/>
+    </row>
+    <row r="23" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B23" s="6">
+        <v>17</v>
+      </c>
+      <c r="D23" s="2" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="24" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="B24" s="2" t="s">
+    <row r="24" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B24" s="6">
+        <v>18</v>
+      </c>
+      <c r="D24" s="2" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="25" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="B25" s="2" t="s">
+    <row r="25" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B25" s="6">
+        <v>19</v>
+      </c>
+      <c r="D25" s="2" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="26" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="B26" s="2" t="s">
+    <row r="26" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B26" s="6">
+        <v>20</v>
+      </c>
+      <c r="D26" s="2" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="27" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A27" s="3" t="s">
+    <row r="27" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A27" s="7">
+        <v>6</v>
+      </c>
+      <c r="B27" s="7"/>
+      <c r="C27" s="3" t="s">
         <v>25</v>
       </c>
-    </row>
-    <row r="28" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="B28" s="2" t="s">
+      <c r="D27" s="2"/>
+    </row>
+    <row r="28" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B28" s="6">
+        <v>21</v>
+      </c>
+      <c r="D28" s="2" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="29" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="B29" s="2" t="s">
+    <row r="29" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B29" s="6">
+        <v>22</v>
+      </c>
+      <c r="D29" s="2" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="30" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="B30" s="2" t="s">
+    <row r="30" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B30" s="6">
+        <v>23</v>
+      </c>
+      <c r="D30" s="2" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="31" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="B31" t="s">
+    <row r="31" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B31" s="6">
+        <v>24</v>
+      </c>
+      <c r="D31" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="32" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A32" s="4" t="s">
+    <row r="32" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A32" s="8">
+        <v>7</v>
+      </c>
+      <c r="B32" s="8"/>
+      <c r="C32" s="4" t="s">
         <v>30</v>
       </c>
-    </row>
-    <row r="33" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B33" s="2" t="s">
+      <c r="D32" s="2"/>
+    </row>
+    <row r="33" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B33" s="6">
+        <v>25</v>
+      </c>
+      <c r="D33" s="2" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="34" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B34" s="2" t="s">
+    <row r="34" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B34" s="6">
+        <v>26</v>
+      </c>
+      <c r="D34" s="2" t="s">
         <v>32</v>
       </c>
     </row>
-    <row r="35" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B35" s="2" t="s">
+    <row r="35" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B35" s="6">
+        <v>27</v>
+      </c>
+      <c r="D35" s="2" t="s">
         <v>33</v>
       </c>
     </row>

</xml_diff>